<commit_message>
Excel exporting works, minor fixes
Exporting to excel works but need some work.
Fixed: function deleting, point spinner value when clear.
</commit_message>
<xml_diff>
--- a/export_to_excel.xlsx
+++ b/export_to_excel.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Documents\GitHub\Carl\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jakub\Documents\GitHub\polynomial_approximation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CC44005-F77A-4B95-A143-77EA237AF873}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F51E154-F1D8-4711-B053-92BED7D91326}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{234F40A1-4E92-4FBE-9E8D-A541D6B14F9E}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Function 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" fullCalcOnLoad="true"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="18">
   <si>
     <t xml:space="preserve">Carl - Universal Polynomial Regression Tool </t>
   </si>
@@ -54,13 +54,40 @@
     <t>Carl output:</t>
   </si>
   <si>
-    <t>Regression degree:</t>
+    <t>This file was automatically generated by Carl</t>
   </si>
   <si>
-    <t>Regression curve:</t>
+    <t>F</t>
   </si>
   <si>
-    <t>This file was automatically generated by Carl</t>
+    <t>u</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>Function curve:</t>
+  </si>
+  <si>
+    <t>Function degree:</t>
+  </si>
+  <si>
+    <t>Function 1</t>
+  </si>
+  <si>
+    <t>y = 2x + (0.33333)</t>
+  </si>
+  <si>
+    <t>Function 2</t>
+  </si>
+  <si>
+    <t>y = (-2.6617e-05)x^5 + (0.0093942)x^4 + (-1.3136)x^3 + (90.9611)x^2 + (-3118.0233)x + (-3118.0233)</t>
   </si>
 </sst>
 </file>
@@ -112,12 +139,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor theme="4" tint="0.59999389629810485"/>
+        <fgColor theme="4" tint="0.59996337778863"/>
+        <bgColor theme="4" tint="0.59996337778863"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -174,53 +201,61 @@
       </bottom>
       <diagonal/>
     </border>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true" applyProtection="true">
+      <protection locked="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center"/>
+      <protection locked="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center"/>
+      <protection locked="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -229,9 +264,9 @@
     <dxf>
       <font>
         <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
+        <strike val="false"/>
+        <outline val="false"/>
+        <shadow val="false"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="12"/>
@@ -240,14 +275,14 @@
         <charset val="238"/>
         <scheme val="none"/>
       </font>
-      <protection locked="0" hidden="0"/>
+      <protection locked="false" hidden="false"/>
     </dxf>
     <dxf>
       <font>
         <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
+        <strike val="false"/>
+        <outline val="false"/>
+        <shadow val="false"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="12"/>
@@ -256,14 +291,14 @@
         <charset val="238"/>
         <scheme val="none"/>
       </font>
-      <protection locked="0" hidden="0"/>
+      <protection locked="false" hidden="false"/>
     </dxf>
     <dxf>
       <font>
         <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
+        <strike val="false"/>
+        <outline val="false"/>
+        <shadow val="false"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="12"/>
@@ -272,14 +307,14 @@
         <charset val="238"/>
         <scheme val="none"/>
       </font>
-      <protection locked="0" hidden="0"/>
+      <protection locked="false" hidden="false"/>
     </dxf>
     <dxf>
       <font>
         <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
+        <strike val="false"/>
+        <outline val="false"/>
+        <shadow val="false"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="12"/>
@@ -288,14 +323,14 @@
         <charset val="238"/>
         <scheme val="none"/>
       </font>
-      <protection locked="0" hidden="0"/>
+      <protection locked="false" hidden="false"/>
     </dxf>
     <dxf>
       <font>
         <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
+        <strike val="false"/>
+        <outline val="false"/>
+        <shadow val="false"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="12"/>
@@ -304,7 +339,7 @@
         <charset val="238"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" justifyLastLine="false" shrinkToFit="false" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -426,6 +461,9 @@
               <c:f>'Function 1'!$E$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Function 1</c:v>
+                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
@@ -471,6 +509,15 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -480,6 +527,15 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -1253,7 +1309,7 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
@@ -1271,7 +1327,7 @@
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+            <a:ext xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0D763445-7A95-434B-8CC0-596AE0F89DB1}"/>
             </a:ext>
           </a:extLst>
@@ -1296,14 +1352,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2AECDC5A-3904-405B-A9B6-7B370F89FEC0}" name="DataTable" displayName="DataTable" ref="A3:C17" totalsRowShown="0" headerRowDxfId="4" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" id="1" name="DataTable" displayName="DataTable" ref="A3:C17" totalsRowShown="false" headerRowDxfId="4" dataDxfId="3" mc:Ignorable="xr xr3" xr:uid="{2AECDC5A-3904-405B-A9B6-7B370F89FEC0}">
   <autoFilter ref="A3:C17" xr:uid="{2AECDC5A-3904-405B-A9B6-7B370F89FEC0}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{30313AC1-6F09-417C-B86F-37A1733762D0}" name="X" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{095D2C13-74B4-4355-A591-3937B7D49090}" name="Y" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{095B9385-006C-42D9-945D-3BE01FFFECE6}" name="σ" dataDxfId="1"/>
+    <tableColumn id="1" name="X" dataDxfId="2" xr3:uid="{30313AC1-6F09-417C-B86F-37A1733762D0}"/>
+    <tableColumn id="2" name="Y" dataDxfId="1" xr3:uid="{095D2C13-74B4-4355-A591-3937B7D49090}"/>
+    <tableColumn id="3" name="σ" dataDxfId="0" xr3:uid="{095B9385-006C-42D9-945D-3BE01FFFECE6}"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="false" showLastColumn="false" showRowStripes="true" showColumnStripes="false"/>
 </table>
 </file>
 
@@ -1604,46 +1660,50 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF836E61-9FFB-48FB-9E75-DADF4A7D8B6C}">
-  <dimension ref="A1:V24"/>
+  <dimension ref="A1:T24"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" zoomScale="109" zoomScaleNormal="109" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView showGridLines="false" showRowColHeaders="false" tabSelected="true" zoomScale="109" zoomScaleNormal="109" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="0.0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="8.88671875" customWidth="1"/>
-    <col min="4" max="4" width="2.21875" customWidth="1"/>
-    <col min="5" max="20" width="8.88671875" customWidth="1"/>
-    <col min="23" max="16384" width="8.88671875" hidden="1"/>
+    <col min="1" max="1" width="4" customWidth="true"/>
+    <col min="3" max="3" width="8.85546875" customWidth="true"/>
+    <col min="4" max="4" width="2.28515625" customWidth="true"/>
+    <col min="5" max="5" width="111.140625" customWidth="true"/>
+    <col min="6" max="20" width="8.85546875" customWidth="true"/>
+    <col min="21" max="22" width="0.0" hidden="true" customWidth="true"/>
+    <col min="23" max="16384" width="8.85546875" hidden="true"/>
+    <col min="2" max="2" width="5.42578125" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="31.2" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="4" t="s">
+    <row r="1" ht="30.75" thickBot="true" x14ac:dyDescent="0.4">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="4"/>
-      <c r="S1" s="4"/>
-      <c r="T1" s="5"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
+      <c r="O1" s="12"/>
+      <c r="P1" s="12"/>
+      <c r="Q1" s="12"/>
+      <c r="R1" s="12"/>
+      <c r="S1" s="12"/>
+      <c r="T1" s="13"/>
     </row>
-    <row r="2" spans="1:20" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" ht="15.75" thickTop="true" x14ac:dyDescent="0.25"/>
+    <row r="3" ht="16.5" thickBot="true" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1653,26 +1713,32 @@
       <c r="C3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="2"/>
-      <c r="G3" s="3"/>
-      <c r="K3" s="2" t="s">
+      <c r="F3" s="6"/>
+      <c r="G3" s="7"/>
+      <c r="K3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="L3" s="2"/>
-      <c r="M3" s="3"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="7"/>
     </row>
-    <row r="4" spans="1:20" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="10"/>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
+    <row r="4" ht="16.5" thickTop="true" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>57</v>
+      </c>
+      <c r="B4" s="2">
+        <v>163</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="E4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
       <c r="K4" s="8"/>
       <c r="L4" s="9"/>
       <c r="M4" s="9"/>
@@ -1683,10 +1749,14 @@
       <c r="R4" s="9"/>
       <c r="S4" s="9"/>
     </row>
-    <row r="5" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="10"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
+    <row r="5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>58</v>
+      </c>
+      <c r="B5" s="2">
+        <v>164</v>
+      </c>
+      <c r="C5" s="2"/>
       <c r="K5" s="8"/>
       <c r="L5" s="9"/>
       <c r="M5" s="9"/>
@@ -1697,15 +1767,19 @@
       <c r="R5" s="9"/>
       <c r="S5" s="9"/>
     </row>
-    <row r="6" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="10"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="E6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F6" s="2"/>
-      <c r="G6" s="3"/>
+    <row r="6" ht="16.5" thickBot="true" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>59</v>
+      </c>
+      <c r="B6" s="2">
+        <v>158</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="E6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="6"/>
+      <c r="G6" s="7"/>
       <c r="K6" s="8"/>
       <c r="L6" s="9"/>
       <c r="M6" s="9"/>
@@ -1716,15 +1790,21 @@
       <c r="R6" s="9"/>
       <c r="S6" s="9"/>
     </row>
-    <row r="7" spans="1:20" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="10"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
+    <row r="7" ht="16.5" thickTop="true" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>62</v>
+      </c>
+      <c r="B7" s="2">
+        <v>175</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="E7" s="4">
+        <v>5</v>
+      </c>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
       <c r="K7" s="8"/>
       <c r="L7" s="9"/>
       <c r="M7" s="9"/>
@@ -1735,10 +1815,14 @@
       <c r="R7" s="9"/>
       <c r="S7" s="9"/>
     </row>
-    <row r="8" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="10"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
+    <row r="8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>63</v>
+      </c>
+      <c r="B8" s="2">
+        <v>171</v>
+      </c>
+      <c r="C8" s="2"/>
       <c r="K8" s="8"/>
       <c r="L8" s="9"/>
       <c r="M8" s="9"/>
@@ -1749,15 +1833,19 @@
       <c r="R8" s="9"/>
       <c r="S8" s="9"/>
     </row>
-    <row r="9" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="10"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="E9" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F9" s="2"/>
-      <c r="G9" s="3"/>
+    <row r="9" ht="16.5" thickBot="true" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
+        <v>64</v>
+      </c>
+      <c r="B9" s="2">
+        <v>172</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="E9" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="6"/>
+      <c r="G9" s="7"/>
       <c r="K9" s="8"/>
       <c r="L9" s="9"/>
       <c r="M9" s="9"/>
@@ -1768,15 +1856,21 @@
       <c r="R9" s="9"/>
       <c r="S9" s="9"/>
     </row>
-    <row r="10" spans="1:20" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="10"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
+    <row r="10" ht="16.5" thickTop="true" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>65</v>
+      </c>
+      <c r="B10" s="2">
+        <v>175</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="E10" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
       <c r="K10" s="8"/>
       <c r="L10" s="9"/>
       <c r="M10" s="9"/>
@@ -1787,10 +1881,14 @@
       <c r="R10" s="9"/>
       <c r="S10" s="9"/>
     </row>
-    <row r="11" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="10"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
+    <row r="11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>68</v>
+      </c>
+      <c r="B11" s="2">
+        <v>165</v>
+      </c>
+      <c r="C11" s="2"/>
       <c r="K11" s="8"/>
       <c r="L11" s="9"/>
       <c r="M11" s="9"/>
@@ -1801,10 +1899,29 @@
       <c r="R11" s="9"/>
       <c r="S11" s="9"/>
     </row>
-    <row r="12" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="10"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
+    <row r="12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>69</v>
+      </c>
+      <c r="B12" s="2">
+        <v>178</v>
+      </c>
+      <c r="C12" s="2"/>
+      <c r="E12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12" t="s">
+        <v>8</v>
+      </c>
+      <c r="G12" t="s">
+        <v>9</v>
+      </c>
+      <c r="H12" t="s">
+        <v>10</v>
+      </c>
+      <c r="I12" t="s">
+        <v>11</v>
+      </c>
       <c r="K12" s="8"/>
       <c r="L12" s="9"/>
       <c r="M12" s="9"/>
@@ -1815,10 +1932,29 @@
       <c r="R12" s="9"/>
       <c r="S12" s="9"/>
     </row>
-    <row r="13" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="10"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
+    <row r="13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>70</v>
+      </c>
+      <c r="B13" s="2">
+        <v>176</v>
+      </c>
+      <c r="C13" s="2"/>
+      <c r="E13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13" t="s">
+        <v>8</v>
+      </c>
+      <c r="G13" t="s">
+        <v>9</v>
+      </c>
+      <c r="H13" t="s">
+        <v>10</v>
+      </c>
+      <c r="I13" t="s">
+        <v>11</v>
+      </c>
       <c r="K13" s="8"/>
       <c r="L13" s="9"/>
       <c r="M13" s="9"/>
@@ -1829,10 +1965,29 @@
       <c r="R13" s="9"/>
       <c r="S13" s="9"/>
     </row>
-    <row r="14" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="10"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
+    <row r="14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>71</v>
+      </c>
+      <c r="B14" s="2">
+        <v>168</v>
+      </c>
+      <c r="C14" s="2"/>
+      <c r="E14" t="s">
+        <v>7</v>
+      </c>
+      <c r="F14" t="s">
+        <v>8</v>
+      </c>
+      <c r="G14" t="s">
+        <v>9</v>
+      </c>
+      <c r="H14" t="s">
+        <v>10</v>
+      </c>
+      <c r="I14" t="s">
+        <v>11</v>
+      </c>
       <c r="K14" s="8"/>
       <c r="L14" s="9"/>
       <c r="M14" s="9"/>
@@ -1843,10 +1998,29 @@
       <c r="R14" s="9"/>
       <c r="S14" s="9"/>
     </row>
-    <row r="15" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A15" s="10"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
+    <row r="15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>81</v>
+      </c>
+      <c r="B15" s="2">
+        <v>183</v>
+      </c>
+      <c r="C15" s="2"/>
+      <c r="E15" t="s">
+        <v>7</v>
+      </c>
+      <c r="F15" t="s">
+        <v>8</v>
+      </c>
+      <c r="G15" t="s">
+        <v>9</v>
+      </c>
+      <c r="H15" t="s">
+        <v>10</v>
+      </c>
+      <c r="I15" t="s">
+        <v>11</v>
+      </c>
       <c r="K15" s="8"/>
       <c r="L15" s="9"/>
       <c r="M15" s="9"/>
@@ -1857,10 +2031,29 @@
       <c r="R15" s="9"/>
       <c r="S15" s="9"/>
     </row>
-    <row r="16" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A16" s="10"/>
-      <c r="B16" s="10"/>
-      <c r="C16" s="10"/>
+    <row r="16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>83</v>
+      </c>
+      <c r="B16" s="2">
+        <v>183</v>
+      </c>
+      <c r="C16" s="2"/>
+      <c r="E16" t="s">
+        <v>7</v>
+      </c>
+      <c r="F16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G16" t="s">
+        <v>9</v>
+      </c>
+      <c r="H16" t="s">
+        <v>10</v>
+      </c>
+      <c r="I16" t="s">
+        <v>11</v>
+      </c>
       <c r="K16" s="8"/>
       <c r="L16" s="9"/>
       <c r="M16" s="9"/>
@@ -1871,10 +2064,29 @@
       <c r="R16" s="9"/>
       <c r="S16" s="9"/>
     </row>
-    <row r="17" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A17" s="10"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
+    <row r="17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>91</v>
+      </c>
+      <c r="B17" s="2">
+        <v>182</v>
+      </c>
+      <c r="C17" s="2"/>
+      <c r="E17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F17" t="s">
+        <v>8</v>
+      </c>
+      <c r="G17" t="s">
+        <v>9</v>
+      </c>
+      <c r="H17" t="s">
+        <v>10</v>
+      </c>
+      <c r="I17" t="s">
+        <v>11</v>
+      </c>
       <c r="K17" s="8"/>
       <c r="L17" s="9"/>
       <c r="M17" s="9"/>
@@ -1885,7 +2097,22 @@
       <c r="R17" s="9"/>
       <c r="S17" s="9"/>
     </row>
-    <row r="18" spans="1:19" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" ht="15.6" customHeight="true" x14ac:dyDescent="0.25">
+      <c r="E18" t="s">
+        <v>7</v>
+      </c>
+      <c r="F18" t="s">
+        <v>8</v>
+      </c>
+      <c r="G18" t="s">
+        <v>9</v>
+      </c>
+      <c r="H18" t="s">
+        <v>10</v>
+      </c>
+      <c r="I18" t="s">
+        <v>11</v>
+      </c>
       <c r="K18" s="8"/>
       <c r="L18" s="9"/>
       <c r="M18" s="9"/>
@@ -1896,7 +2123,22 @@
       <c r="R18" s="9"/>
       <c r="S18" s="9"/>
     </row>
-    <row r="19" spans="1:19" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" ht="15.6" customHeight="true" x14ac:dyDescent="0.25">
+      <c r="E19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F19" t="s">
+        <v>8</v>
+      </c>
+      <c r="G19" t="s">
+        <v>9</v>
+      </c>
+      <c r="H19" t="s">
+        <v>10</v>
+      </c>
+      <c r="I19" t="s">
+        <v>11</v>
+      </c>
       <c r="K19" s="8"/>
       <c r="L19" s="9"/>
       <c r="M19" s="9"/>
@@ -1907,7 +2149,22 @@
       <c r="R19" s="9"/>
       <c r="S19" s="9"/>
     </row>
-    <row r="20" spans="1:19" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" ht="15.6" customHeight="true" x14ac:dyDescent="0.25">
+      <c r="E20" t="s">
+        <v>7</v>
+      </c>
+      <c r="F20" t="s">
+        <v>8</v>
+      </c>
+      <c r="G20" t="s">
+        <v>9</v>
+      </c>
+      <c r="H20" t="s">
+        <v>10</v>
+      </c>
+      <c r="I20" t="s">
+        <v>11</v>
+      </c>
       <c r="K20" s="8"/>
       <c r="L20" s="9"/>
       <c r="M20" s="9"/>
@@ -1918,7 +2175,22 @@
       <c r="R20" s="9"/>
       <c r="S20" s="9"/>
     </row>
-    <row r="21" spans="1:19" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" ht="15.6" customHeight="true" x14ac:dyDescent="0.25">
+      <c r="E21" t="s">
+        <v>7</v>
+      </c>
+      <c r="F21" t="s">
+        <v>8</v>
+      </c>
+      <c r="G21" t="s">
+        <v>9</v>
+      </c>
+      <c r="H21" t="s">
+        <v>10</v>
+      </c>
+      <c r="I21" t="s">
+        <v>11</v>
+      </c>
       <c r="K21" s="8"/>
       <c r="L21" s="9"/>
       <c r="M21" s="9"/>
@@ -1929,7 +2201,22 @@
       <c r="R21" s="9"/>
       <c r="S21" s="9"/>
     </row>
-    <row r="22" spans="1:19" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" ht="15.6" customHeight="true" x14ac:dyDescent="0.25">
+      <c r="E22" t="s">
+        <v>7</v>
+      </c>
+      <c r="F22" t="s">
+        <v>8</v>
+      </c>
+      <c r="G22" t="s">
+        <v>9</v>
+      </c>
+      <c r="H22" t="s">
+        <v>10</v>
+      </c>
+      <c r="I22" t="s">
+        <v>11</v>
+      </c>
       <c r="K22" s="8"/>
       <c r="L22" s="9"/>
       <c r="M22" s="9"/>
@@ -1940,34 +2227,31 @@
       <c r="R22" s="9"/>
       <c r="S22" s="9"/>
     </row>
-    <row r="23" spans="1:19" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="K23" s="6"/>
-      <c r="L23" s="7"/>
-      <c r="M23" s="7"/>
-      <c r="N23" s="7"/>
-      <c r="O23" s="7"/>
-      <c r="P23" s="7"/>
-      <c r="Q23" s="7"/>
-      <c r="R23" s="7"/>
-      <c r="S23" s="7"/>
+    <row r="23" ht="15.6" customHeight="true" x14ac:dyDescent="0.25">
+      <c r="K23" s="10"/>
+      <c r="L23" s="11"/>
+      <c r="M23" s="11"/>
+      <c r="N23" s="11"/>
+      <c r="O23" s="11"/>
+      <c r="P23" s="11"/>
+      <c r="Q23" s="11"/>
+      <c r="R23" s="11"/>
+      <c r="S23" s="11"/>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="S24" s="13" t="s">
-        <v>8</v>
+    <row r="24" x14ac:dyDescent="0.25">
+      <c r="S24" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
-  <mergeCells count="9">
+  <sheetProtection selectLockedCells="true"/>
+  <mergeCells count="6">
     <mergeCell ref="E9:G9"/>
-    <mergeCell ref="E10:I10"/>
     <mergeCell ref="K4:S23"/>
     <mergeCell ref="A1:T1"/>
     <mergeCell ref="E3:G3"/>
     <mergeCell ref="K3:M3"/>
-    <mergeCell ref="E4:I4"/>
     <mergeCell ref="E6:G6"/>
-    <mergeCell ref="E7:I7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>